<commit_message>
updated flight data; added new final feature for aviation
</commit_message>
<xml_diff>
--- a/data/mobility/raw_data/Luftverkehr_Frankfurt_insgesamt_monatlich.xlsx
+++ b/data/mobility/raw_data/Luftverkehr_Frankfurt_insgesamt_monatlich.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christoph\Desktop\3. Semester\Applied Machine Intelligence\Semester Project\Data_preprocessing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christoph\Desktop\3. Semester\Applied Machine Intelligence\Semester Project\Data_preprocessing\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{035F8796-849B-43AF-8556-2D2E5CFA53F9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F76286D6-A810-41AD-91F4-DC00368EB238}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Verkehrsleistung Luftverkehr_Fr" sheetId="1" r:id="rId1"/>
+    <sheet name="46421-0012" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3117" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3018" uniqueCount="41">
   <si>
     <t>GENESIS-Tabelle: 46421-0012</t>
   </si>
@@ -142,13 +142,13 @@
     <t>© Statistisches Bundesamt (Destatis), 2020</t>
   </si>
   <si>
-    <t>Stand: 19.06.2020 / 12:36:47</t>
+    <t>Stand: 06.07.2020 / 15:01:49</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -982,7 +982,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO372"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -41415,14 +41415,14 @@
       <c r="Q334" t="s">
         <v>27</v>
       </c>
-      <c r="R334" t="s">
-        <v>37</v>
-      </c>
-      <c r="S334" t="s">
-        <v>37</v>
+      <c r="R334">
+        <v>1</v>
+      </c>
+      <c r="S334">
+        <v>2</v>
       </c>
       <c r="T334" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="U334" t="s">
         <v>37</v>
@@ -41540,14 +41540,14 @@
       <c r="Q335" t="s">
         <v>27</v>
       </c>
-      <c r="R335" t="s">
-        <v>37</v>
-      </c>
-      <c r="S335" t="s">
-        <v>37</v>
+      <c r="R335">
+        <v>25</v>
+      </c>
+      <c r="S335">
+        <v>54</v>
       </c>
       <c r="T335" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="U335" t="s">
         <v>37</v>
@@ -41665,14 +41665,14 @@
       <c r="Q336">
         <v>0</v>
       </c>
-      <c r="R336" t="s">
-        <v>37</v>
-      </c>
-      <c r="S336" t="s">
-        <v>37</v>
-      </c>
-      <c r="T336" t="s">
-        <v>37</v>
+      <c r="R336">
+        <v>56</v>
+      </c>
+      <c r="S336">
+        <v>112</v>
+      </c>
+      <c r="T336">
+        <v>2</v>
       </c>
       <c r="U336" t="s">
         <v>37</v>
@@ -41790,14 +41790,14 @@
       <c r="Q337" t="s">
         <v>27</v>
       </c>
-      <c r="R337" t="s">
-        <v>37</v>
-      </c>
-      <c r="S337" t="s">
-        <v>37</v>
-      </c>
-      <c r="T337" t="s">
-        <v>37</v>
+      <c r="R337">
+        <v>7</v>
+      </c>
+      <c r="S337">
+        <v>44</v>
+      </c>
+      <c r="T337">
+        <v>0</v>
       </c>
       <c r="U337" t="s">
         <v>37</v>
@@ -41915,14 +41915,14 @@
       <c r="Q338">
         <v>92</v>
       </c>
-      <c r="R338" t="s">
-        <v>37</v>
-      </c>
-      <c r="S338" t="s">
-        <v>37</v>
-      </c>
-      <c r="T338" t="s">
-        <v>37</v>
+      <c r="R338">
+        <v>34</v>
+      </c>
+      <c r="S338">
+        <v>270</v>
+      </c>
+      <c r="T338">
+        <v>83</v>
       </c>
       <c r="U338" t="s">
         <v>37</v>
@@ -42040,14 +42040,14 @@
       <c r="Q339">
         <v>516</v>
       </c>
-      <c r="R339" t="s">
-        <v>37</v>
-      </c>
-      <c r="S339" t="s">
-        <v>37</v>
-      </c>
-      <c r="T339" t="s">
-        <v>37</v>
+      <c r="R339">
+        <v>1272</v>
+      </c>
+      <c r="S339">
+        <v>89706</v>
+      </c>
+      <c r="T339">
+        <v>525</v>
       </c>
       <c r="U339" t="s">
         <v>37</v>
@@ -42165,14 +42165,14 @@
       <c r="Q340">
         <v>1533</v>
       </c>
-      <c r="R340" t="s">
-        <v>37</v>
-      </c>
-      <c r="S340" t="s">
-        <v>37</v>
-      </c>
-      <c r="T340" t="s">
-        <v>37</v>
+      <c r="R340">
+        <v>192</v>
+      </c>
+      <c r="S340">
+        <v>10780</v>
+      </c>
+      <c r="T340">
+        <v>2011</v>
       </c>
       <c r="U340" t="s">
         <v>37</v>
@@ -42290,14 +42290,14 @@
       <c r="Q341">
         <v>65031</v>
       </c>
-      <c r="R341" t="s">
-        <v>37</v>
-      </c>
-      <c r="S341" t="s">
-        <v>37</v>
-      </c>
-      <c r="T341" t="s">
-        <v>37</v>
+      <c r="R341">
+        <v>1965</v>
+      </c>
+      <c r="S341">
+        <v>26099</v>
+      </c>
+      <c r="T341">
+        <v>69740</v>
       </c>
       <c r="U341" t="s">
         <v>37</v>
@@ -42415,14 +42415,14 @@
       <c r="Q342">
         <v>67172</v>
       </c>
-      <c r="R342" t="s">
-        <v>37</v>
-      </c>
-      <c r="S342" t="s">
-        <v>37</v>
-      </c>
-      <c r="T342" t="s">
-        <v>37</v>
+      <c r="R342">
+        <v>3552</v>
+      </c>
+      <c r="S342">
+        <v>127067</v>
+      </c>
+      <c r="T342">
+        <v>72361</v>
       </c>
       <c r="U342" t="s">
         <v>37</v>
@@ -42540,14 +42540,14 @@
       <c r="Q343" t="s">
         <v>27</v>
       </c>
-      <c r="R343" t="s">
-        <v>37</v>
-      </c>
-      <c r="S343" t="s">
-        <v>37</v>
+      <c r="R343">
+        <v>1</v>
+      </c>
+      <c r="S343">
+        <v>2</v>
       </c>
       <c r="T343" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="U343" t="s">
         <v>37</v>
@@ -42665,14 +42665,14 @@
       <c r="Q344" t="s">
         <v>27</v>
       </c>
-      <c r="R344" t="s">
-        <v>37</v>
-      </c>
-      <c r="S344" t="s">
-        <v>37</v>
+      <c r="R344">
+        <v>12</v>
+      </c>
+      <c r="S344">
+        <v>26</v>
       </c>
       <c r="T344" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="U344" t="s">
         <v>37</v>
@@ -42790,14 +42790,14 @@
       <c r="Q345" t="s">
         <v>27</v>
       </c>
-      <c r="R345" t="s">
-        <v>37</v>
-      </c>
-      <c r="S345" t="s">
-        <v>37</v>
+      <c r="R345">
+        <v>41</v>
+      </c>
+      <c r="S345">
+        <v>72</v>
       </c>
       <c r="T345" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="U345" t="s">
         <v>37</v>
@@ -42915,14 +42915,14 @@
       <c r="Q346" t="s">
         <v>27</v>
       </c>
-      <c r="R346" t="s">
-        <v>37</v>
-      </c>
-      <c r="S346" t="s">
-        <v>37</v>
+      <c r="R346">
+        <v>6</v>
+      </c>
+      <c r="S346">
+        <v>45</v>
       </c>
       <c r="T346" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="U346" t="s">
         <v>37</v>
@@ -43040,14 +43040,14 @@
       <c r="Q347">
         <v>11</v>
       </c>
-      <c r="R347" t="s">
-        <v>37</v>
-      </c>
-      <c r="S347" t="s">
-        <v>37</v>
-      </c>
-      <c r="T347" t="s">
-        <v>37</v>
+      <c r="R347">
+        <v>36</v>
+      </c>
+      <c r="S347">
+        <v>211</v>
+      </c>
+      <c r="T347">
+        <v>14</v>
       </c>
       <c r="U347" t="s">
         <v>37</v>
@@ -43165,14 +43165,14 @@
       <c r="Q348">
         <v>381</v>
       </c>
-      <c r="R348" t="s">
-        <v>37</v>
-      </c>
-      <c r="S348" t="s">
-        <v>37</v>
-      </c>
-      <c r="T348" t="s">
-        <v>37</v>
+      <c r="R348">
+        <v>1271</v>
+      </c>
+      <c r="S348">
+        <v>83480</v>
+      </c>
+      <c r="T348">
+        <v>514</v>
       </c>
       <c r="U348" t="s">
         <v>37</v>
@@ -43290,14 +43290,14 @@
       <c r="Q349">
         <v>1495</v>
       </c>
-      <c r="R349" t="s">
-        <v>37</v>
-      </c>
-      <c r="S349" t="s">
-        <v>37</v>
-      </c>
-      <c r="T349" t="s">
-        <v>37</v>
+      <c r="R349">
+        <v>224</v>
+      </c>
+      <c r="S349">
+        <v>19504</v>
+      </c>
+      <c r="T349">
+        <v>2133</v>
       </c>
       <c r="U349" t="s">
         <v>37</v>
@@ -43415,14 +43415,14 @@
       <c r="Q350">
         <v>69008</v>
       </c>
-      <c r="R350" t="s">
-        <v>37</v>
-      </c>
-      <c r="S350" t="s">
-        <v>37</v>
-      </c>
-      <c r="T350" t="s">
-        <v>37</v>
+      <c r="R350">
+        <v>2142</v>
+      </c>
+      <c r="S350">
+        <v>41409</v>
+      </c>
+      <c r="T350">
+        <v>80729</v>
       </c>
       <c r="U350" t="s">
         <v>37</v>
@@ -43540,14 +43540,14 @@
       <c r="Q351">
         <v>70895</v>
       </c>
-      <c r="R351" t="s">
-        <v>37</v>
-      </c>
-      <c r="S351" t="s">
-        <v>37</v>
-      </c>
-      <c r="T351" t="s">
-        <v>37</v>
+      <c r="R351">
+        <v>3733</v>
+      </c>
+      <c r="S351">
+        <v>144749</v>
+      </c>
+      <c r="T351">
+        <v>83390</v>
       </c>
       <c r="U351" t="s">
         <v>37</v>
@@ -43662,14 +43662,14 @@
       <c r="Q352" t="s">
         <v>27</v>
       </c>
-      <c r="R352" t="s">
-        <v>37</v>
-      </c>
-      <c r="S352" t="s">
-        <v>37</v>
+      <c r="R352">
+        <v>2038</v>
+      </c>
+      <c r="S352">
+        <v>122</v>
       </c>
       <c r="T352" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="U352" t="s">
         <v>37</v>
@@ -43784,14 +43784,14 @@
       <c r="Q353">
         <v>0</v>
       </c>
-      <c r="R353" t="s">
-        <v>37</v>
-      </c>
-      <c r="S353" t="s">
-        <v>37</v>
-      </c>
-      <c r="T353" t="s">
-        <v>37</v>
+      <c r="R353">
+        <v>1027</v>
+      </c>
+      <c r="S353">
+        <v>613</v>
+      </c>
+      <c r="T353">
+        <v>0</v>
       </c>
       <c r="U353" t="s">
         <v>37</v>
@@ -43906,14 +43906,14 @@
       <c r="Q354">
         <v>45</v>
       </c>
-      <c r="R354" t="s">
-        <v>37</v>
-      </c>
-      <c r="S354" t="s">
-        <v>37</v>
-      </c>
-      <c r="T354" t="s">
-        <v>37</v>
+      <c r="R354">
+        <v>639</v>
+      </c>
+      <c r="S354">
+        <v>1185</v>
+      </c>
+      <c r="T354">
+        <v>100</v>
       </c>
       <c r="U354" t="s">
         <v>37</v>
@@ -44028,14 +44028,14 @@
       <c r="Q355">
         <v>79</v>
       </c>
-      <c r="R355" t="s">
-        <v>37</v>
-      </c>
-      <c r="S355" t="s">
-        <v>37</v>
-      </c>
-      <c r="T355" t="s">
-        <v>37</v>
+      <c r="R355">
+        <v>107</v>
+      </c>
+      <c r="S355">
+        <v>332</v>
+      </c>
+      <c r="T355">
+        <v>68</v>
       </c>
       <c r="U355" t="s">
         <v>37</v>
@@ -44150,14 +44150,14 @@
       <c r="Q356">
         <v>771</v>
       </c>
-      <c r="R356" t="s">
-        <v>37</v>
-      </c>
-      <c r="S356" t="s">
-        <v>37</v>
-      </c>
-      <c r="T356" t="s">
-        <v>37</v>
+      <c r="R356">
+        <v>242</v>
+      </c>
+      <c r="S356">
+        <v>427</v>
+      </c>
+      <c r="T356">
+        <v>769</v>
       </c>
       <c r="U356" t="s">
         <v>37</v>
@@ -44272,14 +44272,14 @@
       <c r="Q357">
         <v>6777</v>
       </c>
-      <c r="R357" t="s">
-        <v>37</v>
-      </c>
-      <c r="S357" t="s">
-        <v>37</v>
-      </c>
-      <c r="T357" t="s">
-        <v>37</v>
+      <c r="R357">
+        <v>3667</v>
+      </c>
+      <c r="S357">
+        <v>164844</v>
+      </c>
+      <c r="T357">
+        <v>6907</v>
       </c>
       <c r="U357" t="s">
         <v>37</v>
@@ -44394,14 +44394,14 @@
       <c r="Q358">
         <v>33986</v>
       </c>
-      <c r="R358" t="s">
-        <v>37</v>
-      </c>
-      <c r="S358" t="s">
-        <v>37</v>
-      </c>
-      <c r="T358" t="s">
-        <v>37</v>
+      <c r="R358">
+        <v>1901</v>
+      </c>
+      <c r="S358">
+        <v>15238</v>
+      </c>
+      <c r="T358">
+        <v>36908</v>
       </c>
       <c r="U358" t="s">
         <v>37</v>
@@ -44516,14 +44516,14 @@
       <c r="Q359">
         <v>126708</v>
       </c>
-      <c r="R359" t="s">
-        <v>37</v>
-      </c>
-      <c r="S359" t="s">
-        <v>37</v>
-      </c>
-      <c r="T359" t="s">
-        <v>37</v>
+      <c r="R359">
+        <v>3511</v>
+      </c>
+      <c r="S359">
+        <v>29343</v>
+      </c>
+      <c r="T359">
+        <v>133985</v>
       </c>
       <c r="U359" t="s">
         <v>37</v>
@@ -44638,14 +44638,14 @@
       <c r="Q360">
         <v>168366</v>
       </c>
-      <c r="R360" t="s">
-        <v>37</v>
-      </c>
-      <c r="S360" t="s">
-        <v>37</v>
-      </c>
-      <c r="T360" t="s">
-        <v>37</v>
+      <c r="R360">
+        <v>13132</v>
+      </c>
+      <c r="S360">
+        <v>212104</v>
+      </c>
+      <c r="T360">
+        <v>178737</v>
       </c>
       <c r="U360" t="s">
         <v>37</v>
@@ -44760,14 +44760,14 @@
       <c r="Q361" t="s">
         <v>27</v>
       </c>
-      <c r="R361" t="s">
-        <v>37</v>
-      </c>
-      <c r="S361" t="s">
-        <v>37</v>
+      <c r="R361">
+        <v>2033</v>
+      </c>
+      <c r="S361">
+        <v>87</v>
       </c>
       <c r="T361" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="U361" t="s">
         <v>37</v>
@@ -44882,14 +44882,14 @@
       <c r="Q362">
         <v>0</v>
       </c>
-      <c r="R362" t="s">
-        <v>37</v>
-      </c>
-      <c r="S362" t="s">
-        <v>37</v>
+      <c r="R362">
+        <v>992</v>
+      </c>
+      <c r="S362">
+        <v>531</v>
       </c>
       <c r="T362" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="U362" t="s">
         <v>37</v>
@@ -45004,14 +45004,14 @@
       <c r="Q363">
         <v>4</v>
       </c>
-      <c r="R363" t="s">
-        <v>37</v>
-      </c>
-      <c r="S363" t="s">
-        <v>37</v>
-      </c>
-      <c r="T363" t="s">
-        <v>37</v>
+      <c r="R363">
+        <v>626</v>
+      </c>
+      <c r="S363">
+        <v>1313</v>
+      </c>
+      <c r="T363">
+        <v>10</v>
       </c>
       <c r="U363" t="s">
         <v>37</v>
@@ -45126,14 +45126,14 @@
       <c r="Q364">
         <v>49</v>
       </c>
-      <c r="R364" t="s">
-        <v>37</v>
-      </c>
-      <c r="S364" t="s">
-        <v>37</v>
-      </c>
-      <c r="T364" t="s">
-        <v>37</v>
+      <c r="R364">
+        <v>101</v>
+      </c>
+      <c r="S364">
+        <v>309</v>
+      </c>
+      <c r="T364">
+        <v>45</v>
       </c>
       <c r="U364" t="s">
         <v>37</v>
@@ -45248,14 +45248,14 @@
       <c r="Q365">
         <v>569</v>
       </c>
-      <c r="R365" t="s">
-        <v>37</v>
-      </c>
-      <c r="S365" t="s">
-        <v>37</v>
-      </c>
-      <c r="T365" t="s">
-        <v>37</v>
+      <c r="R365">
+        <v>262</v>
+      </c>
+      <c r="S365">
+        <v>386</v>
+      </c>
+      <c r="T365">
+        <v>555</v>
       </c>
       <c r="U365" t="s">
         <v>37</v>
@@ -45370,14 +45370,14 @@
       <c r="Q366">
         <v>5105</v>
       </c>
-      <c r="R366" t="s">
-        <v>37</v>
-      </c>
-      <c r="S366" t="s">
-        <v>37</v>
-      </c>
-      <c r="T366" t="s">
-        <v>37</v>
+      <c r="R366">
+        <v>3776</v>
+      </c>
+      <c r="S366">
+        <v>173720</v>
+      </c>
+      <c r="T366">
+        <v>5989</v>
       </c>
       <c r="U366" t="s">
         <v>37</v>
@@ -45492,14 +45492,14 @@
       <c r="Q367">
         <v>28200</v>
       </c>
-      <c r="R367" t="s">
-        <v>37</v>
-      </c>
-      <c r="S367" t="s">
-        <v>37</v>
-      </c>
-      <c r="T367" t="s">
-        <v>37</v>
+      <c r="R367">
+        <v>1983</v>
+      </c>
+      <c r="S367">
+        <v>33052</v>
+      </c>
+      <c r="T367">
+        <v>33535</v>
       </c>
       <c r="U367" t="s">
         <v>37</v>
@@ -45614,14 +45614,14 @@
       <c r="Q368">
         <v>133373</v>
       </c>
-      <c r="R368" t="s">
-        <v>37</v>
-      </c>
-      <c r="S368" t="s">
-        <v>37</v>
-      </c>
-      <c r="T368" t="s">
-        <v>37</v>
+      <c r="R368">
+        <v>3790</v>
+      </c>
+      <c r="S368">
+        <v>43058</v>
+      </c>
+      <c r="T368">
+        <v>149828</v>
       </c>
       <c r="U368" t="s">
         <v>37</v>
@@ -45736,14 +45736,14 @@
       <c r="Q369">
         <v>167300</v>
       </c>
-      <c r="R369" t="s">
-        <v>37</v>
-      </c>
-      <c r="S369" t="s">
-        <v>37</v>
-      </c>
-      <c r="T369" t="s">
-        <v>37</v>
+      <c r="R369">
+        <v>13563</v>
+      </c>
+      <c r="S369">
+        <v>252456</v>
+      </c>
+      <c r="T369">
+        <v>189962</v>
       </c>
       <c r="U369" t="s">
         <v>37</v>

</xml_diff>